<commit_message>
add excel file to caculate threshold
</commit_message>
<xml_diff>
--- a/wa_threshold.xlsx
+++ b/wa_threshold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\try1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3419F8E0-7EB5-4E54-AA84-2FCE193D4DAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161114B4-8571-484A-B4B0-846AF8DB82E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{AE127A0F-4DEA-4AF2-95EC-3B73EF64199E}"/>
   </bookViews>
@@ -76,16 +76,8 @@
 最多能有多少重复签名</t>
   </si>
   <si>
-    <t>提交的签名中
-最多能有多少重复签名 x 采样率</t>
-  </si>
-  <si>
     <t>采样的样本中
 最多能有多少重复签名的上界</t>
-  </si>
-  <si>
-    <t>采样的样本中
-能有多少重复签名</t>
   </si>
   <si>
     <t>采样的样本中能有多少重复签名
@@ -103,6 +95,26 @@
   </si>
   <si>
     <t>&gt;10%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">提交的签名中
+最多能有多少重复签名 x 采样率 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x 采样率</t>
+    </r>
+  </si>
+  <si>
+    <t>采样的样本中
+能有多少对重复签名</t>
   </si>
 </sst>
 </file>
@@ -112,10 +124,17 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,8 +211,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +530,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,9 +588,14 @@
       <c r="O1" s="2">
         <v>130000</v>
       </c>
-      <c r="R1">
-        <f>19*5-87</f>
-        <v>8</v>
+      <c r="P1" s="2">
+        <v>130000</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>130000</v>
+      </c>
+      <c r="R1" s="2">
+        <v>130000</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -618,6 +642,15 @@
       <c r="O2" s="10">
         <v>177000</v>
       </c>
+      <c r="P2" s="10">
+        <v>200000</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>195000</v>
+      </c>
+      <c r="R2" s="10">
+        <v>192500</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -663,6 +696,15 @@
       <c r="O3" s="3">
         <v>0.03</v>
       </c>
+      <c r="P3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -723,13 +765,25 @@
         <f>O$2*O$3</f>
         <v>5310</v>
       </c>
+      <c r="P4" s="2">
+        <f>P$2*P$3</f>
+        <v>6000</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>Q$2*Q$3</f>
+        <v>5850</v>
+      </c>
+      <c r="R4" s="2">
+        <f>R$2*R$3</f>
+        <v>5775</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>0.7</v>
@@ -750,25 +804,34 @@
         <v>0.8</v>
       </c>
       <c r="I5" s="11">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="J5" s="11">
-        <v>0.68799999999999994</v>
+        <v>0.75</v>
       </c>
       <c r="K5" s="11">
-        <v>0.65300000000000002</v>
+        <v>0.74</v>
       </c>
       <c r="L5" s="11">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="M5" s="1">
         <v>0.75</v>
       </c>
       <c r="N5" s="11">
-        <v>0.69399999999999995</v>
+        <v>0.8</v>
       </c>
       <c r="O5" s="11">
-        <v>0.74</v>
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -804,19 +867,19 @@
       </c>
       <c r="I6" s="2">
         <f>I$2*(1-I$5)</f>
-        <v>55950.000000000007</v>
+        <v>46625</v>
       </c>
       <c r="J6" s="2">
         <f>J$2*(1-J$5)</f>
-        <v>59280.000000000007</v>
+        <v>47500</v>
       </c>
       <c r="K6" s="2">
         <f>K$2*(1-K$5)</f>
-        <v>69400</v>
+        <v>52000</v>
       </c>
       <c r="L6" s="2">
         <f>L$2*(1-L$5)</f>
-        <v>43500</v>
+        <v>34799.999999999993</v>
       </c>
       <c r="M6" s="2">
         <f>M$2*(1-M$5)</f>
@@ -824,11 +887,23 @@
       </c>
       <c r="N6" s="2">
         <f>N$2*(1-N$5)</f>
-        <v>58140.000000000007</v>
+        <v>37999.999999999993</v>
       </c>
       <c r="O6" s="2">
         <f>O$2*(1-O$5)</f>
-        <v>46020</v>
+        <v>35399.999999999993</v>
+      </c>
+      <c r="P6" s="2">
+        <f>P$2*(1-P$5)</f>
+        <v>50000</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>Q$2*(1-Q$5)</f>
+        <v>48750</v>
+      </c>
+      <c r="R6" s="2">
+        <f>R$2*(1-R$5)</f>
+        <v>48125</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -864,19 +939,19 @@
       </c>
       <c r="I7" s="2">
         <f>I$6+1.5*SQRT(I$6)</f>
-        <v>56304.806285175451</v>
+        <v>46948.892343225336</v>
       </c>
       <c r="J7" s="2">
         <f>J$6+1.5*SQRT(J$6)</f>
-        <v>59645.212267044801</v>
+        <v>47826.917420765552</v>
       </c>
       <c r="K7" s="2">
         <f>K$6+1.5*SQRT(K$6)</f>
-        <v>69795.158196169592</v>
+        <v>52342.052627529738</v>
       </c>
       <c r="L7" s="2">
         <f>L$6+1.5*SQRT(L$6)</f>
-        <v>43812.849804219215</v>
+        <v>35079.821371592654</v>
       </c>
       <c r="M7" s="2">
         <f>M$6+1.5*SQRT(M$6)</f>
@@ -884,11 +959,23 @@
       </c>
       <c r="N7" s="2">
         <f>N$6+1.5*SQRT(N$6)</f>
-        <v>58501.683563353392</v>
+        <v>38292.403830344265</v>
       </c>
       <c r="O7" s="2">
         <f>O$6+1.5*SQRT(O$6)</f>
-        <v>46341.784089103239</v>
+        <v>35682.223315833391</v>
+      </c>
+      <c r="P7" s="2">
+        <f>P$6+1.5*SQRT(P$6)</f>
+        <v>50335.410196624965</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>Q$6+1.5*SQRT(Q$6)</f>
+        <v>49081.191032487295</v>
+      </c>
+      <c r="R7" s="2">
+        <f>R$6+1.5*SQRT(R$6)</f>
+        <v>48454.061164527207</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -924,19 +1011,19 @@
       </c>
       <c r="I8" s="2">
         <f>I2-I1-I7</f>
-        <v>195.19371482454881</v>
+        <v>9551.1076567746641</v>
       </c>
       <c r="J8" s="2">
         <f>J2-J1-J7</f>
-        <v>354.78773295519932</v>
+        <v>12173.082579234448</v>
       </c>
       <c r="K8" s="2">
         <f>K2-K1-K7</f>
-        <v>204.84180383040803</v>
+        <v>17657.947372470262</v>
       </c>
       <c r="L8" s="2">
         <f>L2-L1-L7</f>
-        <v>187.150195780785</v>
+        <v>8920.178628407346</v>
       </c>
       <c r="M8" s="2">
         <f>M2-M1-M7</f>
@@ -944,19 +1031,31 @@
       </c>
       <c r="N8" s="2">
         <f>N2-N1-N7</f>
-        <v>1498.3164366466081</v>
+        <v>21707.596169655735</v>
       </c>
       <c r="O8" s="2">
         <f>O2-O1-O7</f>
-        <v>658.21591089676076</v>
+        <v>11317.776684166609</v>
+      </c>
+      <c r="P8" s="2">
+        <f>P2-P1-P7</f>
+        <v>19664.589803375035</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>Q2-Q1-Q7</f>
+        <v>15918.808967512705</v>
+      </c>
+      <c r="R8" s="2">
+        <f>R2-R1-R7</f>
+        <v>14045.938835472793</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <f>C$8*C$3</f>
@@ -983,40 +1082,52 @@
         <v>651.22788508967199</v>
       </c>
       <c r="I9" s="2">
-        <f>I$8*I$3</f>
-        <v>5.8558114447364638</v>
+        <f>I$8*I$3*I$3</f>
+        <v>8.5959968910971973</v>
       </c>
       <c r="J9" s="2">
-        <f>J$8*J$3</f>
-        <v>10.643631988655979</v>
+        <f t="shared" ref="J9:R9" si="0">J$8*J$3*J$3</f>
+        <v>10.955774321311003</v>
       </c>
       <c r="K9" s="2">
-        <f>K$8*K$3</f>
-        <v>6.1452541149122402</v>
+        <f t="shared" si="0"/>
+        <v>15.892152635223235</v>
       </c>
       <c r="L9" s="2">
-        <f>L$8*L$3</f>
-        <v>5.6145058734235498</v>
+        <f t="shared" si="0"/>
+        <v>8.0281607655666107</v>
       </c>
       <c r="M9" s="2">
-        <f>M$8*M$3</f>
-        <v>365.19247737703341</v>
+        <f t="shared" si="0"/>
+        <v>10.955774321311003</v>
       </c>
       <c r="N9" s="2">
-        <f>N$8*N$3</f>
-        <v>44.949493099398239</v>
+        <f t="shared" si="0"/>
+        <v>19.536836552690158</v>
       </c>
       <c r="O9" s="2">
-        <f>O$8*O$3</f>
-        <v>19.746477326902824</v>
+        <f t="shared" si="0"/>
+        <v>10.185999015749948</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="0"/>
+        <v>17.69813082303753</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>14.326928070761433</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="0"/>
+        <v>12.641344951925513</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C10" s="2">
         <f>C$9-1.65*SQRT(C$9)</f>
@@ -1044,36 +1155,48 @@
       </c>
       <c r="I10" s="2">
         <f>I$9-1.65*SQRT(I$9)</f>
-        <v>1.8630120936176247</v>
+        <v>3.7583733489008724</v>
       </c>
       <c r="J10" s="2">
         <f>J$9-1.65*SQRT(J$9)</f>
-        <v>5.2605763425460585</v>
+        <v>5.4943554956056158</v>
       </c>
       <c r="K10" s="2">
         <f>K$9-1.65*SQRT(K$9)</f>
-        <v>2.0549663098979556</v>
+        <v>9.3144337639582702</v>
       </c>
       <c r="L10" s="2">
         <f>L$9-1.65*SQRT(L$9)</f>
-        <v>1.7048393607404519</v>
+        <v>3.3530492498640072</v>
       </c>
       <c r="M10" s="2">
         <f>M$9-1.65*SQRT(M$9)</f>
-        <v>333.66096108525045</v>
+        <v>5.4943554956056158</v>
       </c>
       <c r="N10" s="2">
         <f>N$9-1.65*SQRT(N$9)</f>
-        <v>33.887169882139048</v>
+        <v>12.243755069894361</v>
       </c>
       <c r="O10" s="2">
         <f>O$9-1.65*SQRT(O$9)</f>
-        <v>12.414370909065386</v>
+        <v>4.9199395477625956</v>
+      </c>
+      <c r="P10" s="2">
+        <f>P$9-1.65*SQRT(P$9)</f>
+        <v>10.756721660214779</v>
+      </c>
+      <c r="Q10" s="2">
+        <f>Q$9-1.65*SQRT(Q$9)</f>
+        <v>8.0815248273632925</v>
+      </c>
+      <c r="R10" s="2">
+        <f>R$9-1.65*SQRT(R$9)</f>
+        <v>6.7748245495390007</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7">
@@ -1081,64 +1204,72 @@
         <v>4.3488066330539699E-2</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" ref="D11:O11" si="0">D$10/D$4</f>
+        <f t="shared" ref="D11:Q11" si="1">D$10/D$4</f>
         <v>1.132756087948196E-2</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7239713729133557E-3</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2539035258413564E-3</v>
       </c>
       <c r="G11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14029135364387041</v>
       </c>
       <c r="H11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10686337886254943</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="0"/>
-        <v>3.3297803281816349E-4</v>
+        <f t="shared" si="1"/>
+        <v>6.7173786396798434E-4</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="0"/>
-        <v>9.229081302712383E-4</v>
+        <f t="shared" si="1"/>
+        <v>9.6392201677291507E-4</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="0"/>
-        <v>3.4249438498299258E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.5524056273263783E-3</v>
       </c>
       <c r="L11" s="7">
-        <f t="shared" si="0"/>
-        <v>3.2659757868591031E-4</v>
+        <f t="shared" si="1"/>
+        <v>6.4234659959080595E-4</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" si="0"/>
-        <v>5.8537010716710608E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.6392201677291507E-4</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" si="0"/>
-        <v>5.9451175231822889E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.1480272052446245E-3</v>
       </c>
       <c r="O11" s="7">
-        <f t="shared" si="0"/>
-        <v>2.3379229583927281E-3</v>
+        <f t="shared" si="1"/>
+        <v>9.2654228771423648E-4</v>
+      </c>
+      <c r="P11" s="7">
+        <f t="shared" si="1"/>
+        <v>1.79278694336913E-3</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" si="1"/>
+        <v>1.3814572354467166E-3</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J13" s="8"/>
       <c r="L13" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>